<commit_message>
Update development plan for sprint 3
</commit_message>
<xml_diff>
--- a/docs/迭代开发计划.xlsx
+++ b/docs/迭代开发计划.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Use Cases" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="151">
   <si>
     <t xml:space="preserve">Use Case ID</t>
   </si>
@@ -257,6 +257,10 @@
     <t xml:space="preserve">前端在调用服务器API时，可以在后端创建用户账户</t>
   </si>
   <si>
+    <t xml:space="preserve">- 后端应当按照API要求接受前端请求
+- 后端应在创建请求非法（用户名重复等）情况下返回创建失败的响应</t>
+  </si>
+  <si>
     <t xml:space="preserve">HR房间信息组件</t>
   </si>
   <si>
@@ -297,16 +301,47 @@
     <t xml:space="preserve">前端在调用API时，管理后台创建房间数据</t>
   </si>
   <si>
+    <t xml:space="preserve">- 请求合法时，后端应创建房间并写入数据库
+- 请求者无权限时，后端应返回失败响应</t>
+  </si>
+  <si>
     <t xml:space="preserve">后端设置房间</t>
   </si>
   <si>
     <t xml:space="preserve">前端在调用API时，管理后台设置房间名、企业 LOGO</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- 前端请求更改相应项目时，后端应当更改数据库数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- 请求者无权限时，后端应返回失败响应</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">后端邀请主考官</t>
   </si>
   <si>
     <t xml:space="preserve">前端在调用API时，后台将主考官加入房间，并发送邀请邮件给主考官</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- 后端应按照API，将主考官数据关联到房间
+- 后端应当给主考官发送邀请邮件
+- 后端应当对非法请求返回失败响应</t>
   </si>
   <si>
     <t xml:space="preserve">候选人管理界面</t>
@@ -473,7 +508,7 @@
     <t xml:space="preserve">面试官点击「面试结束」，并选择「通过」或「未通过」</t>
   </si>
   <si>
-    <t xml:space="preserve">面试者信息页</t>
+    <t xml:space="preserve">面试官房间面试者信息页</t>
   </si>
   <si>
     <t xml:space="preserve">面试官可以查看房间中的面试者</t>
@@ -483,7 +518,7 @@
 - 没有候选人时，显示“暂无候选人”字样</t>
   </si>
   <si>
-    <t xml:space="preserve">面试者面试结果</t>
+    <t xml:space="preserve">面试官查看面试结果</t>
   </si>
   <si>
     <t xml:space="preserve">面试官点击房间中面试者，可以查看面试结果</t>
@@ -495,6 +530,12 @@
     <t xml:space="preserve">面试结束后，HR 可以在系统管理后台下载某位候选人的面试记录，面试官可以在房间管理后台下载某位候选人的面试记录</t>
   </si>
   <si>
+    <t xml:space="preserve">用户登入登出</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HR、面试者和面试官可以通过这一后台登录或登出面试系统</t>
+  </si>
+  <si>
     <t xml:space="preserve">Author</t>
   </si>
   <si>
@@ -540,22 +581,67 @@
     <t xml:space="preserve">F_5</t>
   </si>
   <si>
+    <t xml:space="preserve">叶方轲</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_39</t>
+  </si>
+  <si>
     <t xml:space="preserve">莫宇尘</t>
   </si>
   <si>
+    <t xml:space="preserve">Estimated Effot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_37</t>
+  </si>
+  <si>
     <t xml:space="preserve">F_9</t>
   </si>
   <si>
-    <t xml:space="preserve">叶方轲</t>
-  </si>
-  <si>
     <t xml:space="preserve">F_10</t>
   </si>
   <si>
     <t xml:space="preserve">F_11</t>
   </si>
   <si>
-    <t xml:space="preserve">Estimated Effot</t>
+    <t xml:space="preserve">F_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_28</t>
   </si>
 </sst>
 </file>
@@ -669,7 +755,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -722,10 +808,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -747,15 +829,15 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8604651162791"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="99.8046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="102.758139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -857,21 +939,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="18.4604651162791"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="18.5813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="18.4604651162791"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="18.953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="79.6232558139535"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="69.6511627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="18.953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="19.2"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="18.953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="19.5674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="81.9581395348837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="71.7441860465116"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -970,7 +1052,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="36.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_5</v>
@@ -985,7 +1067,9 @@
       <c r="E6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="0"/>
+      <c r="F6" s="11" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="87.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="str">
@@ -996,17 +1080,17 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D7" s="0"/>
       <c r="E7" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="70.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="70.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_7</v>
@@ -1015,17 +1099,17 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D8" s="0"/>
       <c r="E8" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="87.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="87.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_8</v>
@@ -1034,17 +1118,17 @@
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" s="0"/>
       <c r="E9" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_9</v>
@@ -1053,14 +1137,17 @@
         <v>5</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_10</v>
@@ -1069,14 +1156,17 @@
         <v>5</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_11</v>
@@ -1085,14 +1175,17 @@
         <v>5</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="53.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_12</v>
@@ -1101,17 +1194,17 @@
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D13" s="0"/>
       <c r="E13" s="4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="36.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_13</v>
@@ -1120,17 +1213,17 @@
         <v>13</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D14" s="0"/>
       <c r="E14" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="70.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="70.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_14</v>
@@ -1139,17 +1232,17 @@
         <v>7</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D15" s="0"/>
       <c r="E15" s="4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="70.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="70.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_15</v>
@@ -1158,14 +1251,14 @@
         <v>7</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D16" s="0"/>
       <c r="E16" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1177,12 +1270,13 @@
         <v>7</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="12" t="s">
-        <v>63</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="str">
@@ -1193,12 +1287,13 @@
         <v>7</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="12" t="s">
-        <v>65</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="str">
@@ -1209,12 +1304,13 @@
         <v>7</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="12" t="s">
-        <v>67</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="str">
@@ -1225,12 +1321,13 @@
         <v>7</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12" t="s">
-        <v>69</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="str">
@@ -1241,12 +1338,13 @@
         <v>9</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D21" s="0"/>
       <c r="E21" s="0" t="s">
-        <v>71</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="str">
@@ -1257,12 +1355,13 @@
         <v>9</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D22" s="0"/>
       <c r="E22" s="0" t="s">
-        <v>73</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="str">
@@ -1273,12 +1372,13 @@
         <v>9</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D23" s="0"/>
       <c r="E23" s="0" t="s">
-        <v>75</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="str">
@@ -1289,12 +1389,13 @@
         <v>9</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D24" s="0"/>
       <c r="E24" s="0" t="s">
-        <v>77</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="str">
@@ -1305,12 +1406,13 @@
         <v>9</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D25" s="0"/>
       <c r="E25" s="0" t="s">
-        <v>79</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="str">
@@ -1321,12 +1423,13 @@
         <v>9</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="12" t="s">
-        <v>81</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="str">
@@ -1337,12 +1440,13 @@
         <v>9</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="12" t="s">
-        <v>83</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="str">
@@ -1353,12 +1457,13 @@
         <v>9</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="12" t="s">
-        <v>85</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="str">
@@ -1369,12 +1474,13 @@
         <v>9</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="12" t="s">
-        <v>87</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="F29" s="11"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="str">
@@ -1385,12 +1491,13 @@
         <v>11</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="12" t="s">
-        <v>89</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="F30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="str">
@@ -1401,12 +1508,13 @@
         <v>11</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="12" t="s">
-        <v>91</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="F31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="str">
@@ -1417,12 +1525,13 @@
         <v>11</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12" t="s">
-        <v>93</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="F32" s="11"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="str">
@@ -1433,12 +1542,13 @@
         <v>11</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="12" t="s">
-        <v>95</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="F33" s="11"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="str">
@@ -1449,12 +1559,13 @@
         <v>11</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="12" t="s">
-        <v>97</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="F34" s="11"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="str">
@@ -1465,12 +1576,13 @@
         <v>11</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="12" t="s">
-        <v>99</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="F35" s="11"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="str">
@@ -1481,14 +1593,15 @@
         <v>11</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>105</v>
+      </c>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="37" customFormat="false" ht="36.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_36</v>
@@ -1497,14 +1610,14 @@
         <v>13</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D37" s="0"/>
       <c r="E37" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="36.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,14 +1629,14 @@
         <v>13</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D38" s="0"/>
       <c r="E38" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="F38" s="13" t="s">
-        <v>55</v>
+        <v>110</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1535,12 +1648,29 @@
         <v>13</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="12" t="s">
-        <v>108</v>
-      </c>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="str">
+        <f aca="false">"F_"&amp;(ROW()-1)</f>
+        <v>F_39</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" s="0"/>
+      <c r="E40" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="F40" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1566,13 +1696,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4604651162791"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.1209302325581"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.7209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8604651162791"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.4604651162791"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1583,16 +1713,16 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1624,21 +1754,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="24.9813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8883720930233"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.506976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.153488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1649,27 +1779,27 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="D2" s="9" t="n">
         <v>4</v>
@@ -1677,13 +1807,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D3" s="9" t="n">
         <v>2</v>
@@ -1691,13 +1821,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="D4" s="9" t="n">
         <v>4</v>
@@ -1705,13 +1835,13 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D5" s="9" t="n">
         <v>4</v>
@@ -1719,13 +1849,13 @@
     </row>
     <row r="6" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D6" s="9" t="n">
         <v>4</v>
@@ -1733,13 +1863,13 @@
     </row>
     <row r="7" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D7" s="9" t="n">
         <v>3</v>
@@ -1747,13 +1877,13 @@
     </row>
     <row r="8" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>116</v>
       </c>
       <c r="D8" s="9" t="n">
         <v>3</v>
@@ -1764,58 +1894,36 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="B10" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D10" s="9" t="n">
         <v>4</v>
       </c>
+      <c r="E10" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>44</v>
+        <v>131</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D11" s="9" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="D12" s="9" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" s="9" t="n">
-        <v>4</v>
+      <c r="E11" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1837,18 +1945,18 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.9023255813953"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8744186046512"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.2604651162791"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.5674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.306976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.4883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8744186046512"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1859,104 +1967,255 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>134</v>
+      </c>
       <c r="B2" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>125</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>135</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>125</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>136</v>
+      </c>
       <c r="B4" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>122</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>137</v>
+      </c>
       <c r="B5" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>122</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>138</v>
+      </c>
       <c r="B6" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>139</v>
+      </c>
       <c r="B7" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="12" t="s">
-        <v>62</v>
-      </c>
+      <c r="A9" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="12" t="s">
-        <v>64</v>
+      <c r="A10" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="12" t="s">
+      <c r="C12" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="s">
-        <v>80</v>
+      <c r="C13" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="s">
-        <v>82</v>
+      <c r="A14" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12" t="s">
+      <c r="A15" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12" t="s">
+      <c r="C16" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>86</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>1.5</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1991,7 +2250,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2002,86 +2261,86 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="12" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="12" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="12" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="12" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="12" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="12" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="12" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="12" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update development plan for sprint 4
</commit_message>
<xml_diff>
--- a/docs/迭代开发计划.xlsx
+++ b/docs/迭代开发计划.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Use Cases" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="185">
   <si>
     <t xml:space="preserve">Use Case ID</t>
   </si>
@@ -181,7 +181,7 @@
 - 调用服务器API失败时，应当显示提示信息；成功则跳转到登陆页</t>
   </si>
   <si>
-    <t xml:space="preserve">登陆页</t>
+    <t xml:space="preserve">登录页</t>
   </si>
   <si>
     <r>
@@ -311,26 +311,8 @@
     <t xml:space="preserve">前端在调用API时，管理后台设置房间名、企业 LOGO</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- 前端请求更改相应项目时，后端应当更改数据库数据
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- 请求者无权限时，后端应返回失败响应</t>
-    </r>
+    <t xml:space="preserve">- 前端请求更改相应项目时，后端应当更改数据库数据
+- 请求者无权限时，后端应返回失败响应</t>
   </si>
   <si>
     <t xml:space="preserve">后端邀请主考官</t>
@@ -394,118 +376,191 @@
     <t xml:space="preserve">HR 在系统管理后台添加 / 导入候选人</t>
   </si>
   <si>
+    <t xml:space="preserve">- 当前端请求到达时，后端可以将候选人信息加入数据库，并向前端返回添加结果
+- 当前端要求批量添加候选人时，后端应当能准确无误添加所有候选人</t>
+  </si>
+  <si>
     <t xml:space="preserve">查看候选人后端</t>
   </si>
   <si>
     <t xml:space="preserve">HR、面试官查看候选人信息</t>
   </si>
   <si>
+    <t xml:space="preserve">- 前端请求某一候选人信息时，后端按照候选人id返回候选人信息
+- 前端请求某一房间全部候选人时，后端按照偏置，数量限制等参数返回候选人列表</t>
+  </si>
+  <si>
     <t xml:space="preserve">分配候选人后端</t>
   </si>
   <si>
     <t xml:space="preserve">HR 将候选人分配到不同的面试房间并发送邀请邮件给候选人</t>
   </si>
   <si>
+    <t xml:space="preserve">- 前端点击发送邮件按钮并请求后端后，后端应当为面试者创建账号，并将含账号信息的邮件发送到面试者邮箱</t>
+  </si>
+  <si>
     <t xml:space="preserve">查看结果后端</t>
   </si>
   <si>
     <t xml:space="preserve">HR、主考官可以查看候选人的状态为通过 / 未通过 / 未面试</t>
   </si>
   <si>
+    <t xml:space="preserve">- 后端按照前端请求，返回面试的白板，代码，视频，报告记录</t>
+  </si>
+  <si>
     <t xml:space="preserve">创建面试题页</t>
   </si>
   <si>
     <t xml:space="preserve">主考官点击创建面试题，可以打开创建面试题页</t>
   </si>
   <si>
+    <t xml:space="preserve">- 本页面应当能显示所有已有的面试题
+- 本页面应当具有添加题目按钮，并按照分类导航到选择、填空、简答、代码题创建页</t>
+  </si>
+  <si>
     <t xml:space="preserve">选择题组件</t>
   </si>
   <si>
     <t xml:space="preserve">主考官可以在选择题组件处编辑选择题</t>
   </si>
   <si>
+    <t xml:space="preserve">- 本组件可显示选择题题目，题目描述，以及选项
+- 本组件应当对选项进行验证，不能允许重复选项，并对选项上限做出限制
+- 本组件应当可以指定一个或多个正确选项</t>
+  </si>
+  <si>
     <t xml:space="preserve">填空题组件</t>
   </si>
   <si>
     <t xml:space="preserve">主考官可以在填空题组件处编辑填空题</t>
   </si>
   <si>
+    <t xml:space="preserve">- 本组件应当能显示并编辑填空题题目及内容</t>
+  </si>
+  <si>
     <t xml:space="preserve">简答题组件</t>
   </si>
   <si>
     <t xml:space="preserve">主考官可以在简答题组件处编辑简答题</t>
   </si>
   <si>
+    <t xml:space="preserve">- 本组件应当能显示并编辑简答题题目及内容</t>
+  </si>
+  <si>
     <t xml:space="preserve">编程题组件</t>
   </si>
   <si>
     <t xml:space="preserve">主考官可以在编程题组件处编辑编程题</t>
   </si>
   <si>
+    <t xml:space="preserve">- 本组件应当能显示并编辑编程题的题目、内容以及样例输入输出</t>
+  </si>
+  <si>
     <t xml:space="preserve">设置选择题后端</t>
   </si>
   <si>
     <t xml:space="preserve">主考官可以提前添加面试过程中会用到的选择题</t>
   </si>
   <si>
+    <t xml:space="preserve">- 后端应当按照前端传来的数据，设置选择题，将其关联到面试房间
+- 后端应当能按照前端请求返回题目，且保证返回题目的选项顺序与添加时一致</t>
+  </si>
+  <si>
     <t xml:space="preserve">设置填空题后端</t>
   </si>
   <si>
     <t xml:space="preserve">主考官可以提前添加面试过程中会用到的填空题</t>
   </si>
   <si>
+    <t xml:space="preserve">- 后端应当按照前端传来的数据，设置填空题，将其关联到面试房间
+- 后端应当能按照前端请求返回题目</t>
+  </si>
+  <si>
     <t xml:space="preserve">设置简答题后端</t>
   </si>
   <si>
     <t xml:space="preserve">主考官可以提前添加面试过程中会用到的简答题</t>
   </si>
   <si>
+    <t xml:space="preserve">- 后端应当按照前端传来的数据，设置简答题，将其关联到面试房间
+- 后端应当能按照前端请求返回题目</t>
+  </si>
+  <si>
     <t xml:space="preserve">设置编程题后端</t>
   </si>
   <si>
     <t xml:space="preserve">主考官可以提前添加面试过程中会用到的编程题</t>
   </si>
   <si>
+    <t xml:space="preserve">- 后端应当按照前端传来的数据，设置编程题，将其关联到面试房间
+- 后端应当能按照前端请求返回题目</t>
+  </si>
+  <si>
     <t xml:space="preserve">候选人排队后端</t>
   </si>
   <si>
     <t xml:space="preserve">候选人进入房间后排队等待面试</t>
   </si>
   <si>
+    <t xml:space="preserve">- 前端进行调用时，后端可返回本场面试的候选人，以及它们的信息和状态
+- 当候选人超时，前端调用超时API时，后端可改变候选人状态，并将候选人移动到队列末尾</t>
+  </si>
+  <si>
     <t xml:space="preserve">通知面试开始后端</t>
   </si>
   <si>
     <t xml:space="preserve">主考官点击「面试开始」，发送短信通知排在候选人列表中第一位的候选人</t>
   </si>
   <si>
+    <t xml:space="preserve">- 前端选择开始面试时，后端可以将所有到场的候选人加入面试，并向前端返回信息</t>
+  </si>
+  <si>
     <t xml:space="preserve">获取面试题后端</t>
   </si>
   <si>
     <t xml:space="preserve">面试官使用的面试题会被插入到聊天室中，候选人根据题目在聊天室、白板、代码协同编辑作答或口头作答</t>
   </si>
   <si>
+    <t xml:space="preserve">- 前端按照房间获取面试题时，后端应当可以按照添加题目的顺序返回所有面试题</t>
+  </si>
+  <si>
     <t xml:space="preserve">视频传输后端</t>
   </si>
   <si>
     <t xml:space="preserve">面试官与候选人使用视频并产生记录</t>
   </si>
   <si>
+    <t xml:space="preserve">- 后端应当可以处理面试官与候选人的实时视频连接
+- 后端应当可以保存面试过程中的视频
+- 后端在前端请求视频记录时，应当可以返回视频的下载链接</t>
+  </si>
+  <si>
     <t xml:space="preserve">非视频传输后端</t>
   </si>
   <si>
     <t xml:space="preserve">面试官与候选人使用白板、代码协同编辑、聊天室并产生记录</t>
   </si>
   <si>
+    <t xml:space="preserve">- 后端应当可以记录前端传来的白板、代码、聊天记录</t>
+  </si>
+  <si>
     <t xml:space="preserve">添加面试报告后端</t>
   </si>
   <si>
     <t xml:space="preserve">面试官随时撰写面试报告</t>
   </si>
   <si>
+    <t xml:space="preserve">- 面试官撰写面试报告时，后端可以随时更新报告状态
+- 后端在面试结束后生成最终版本报告，并可以在前端请求时返回报告下载链接</t>
+  </si>
+  <si>
     <t xml:space="preserve">结束面试后端</t>
   </si>
   <si>
     <t xml:space="preserve">面试官点击「面试结束」，并选择「通过」或「未通过」</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- 后端在前端设置面试通过状态时，更新候选人信息</t>
   </si>
   <si>
     <t xml:space="preserve">面试官房间面试者信息页</t>
@@ -530,12 +585,30 @@
     <t xml:space="preserve">面试结束后，HR 可以在系统管理后台下载某位候选人的面试记录，面试官可以在房间管理后台下载某位候选人的面试记录</t>
   </si>
   <si>
+    <t xml:space="preserve">- 面试结束后，后端应在前端进行请求时，返回面试的视频、白板、代码、聊天信息</t>
+  </si>
+  <si>
     <t xml:space="preserve">用户登入登出</t>
   </si>
   <si>
     <t xml:space="preserve">HR、面试者和面试官可以通过这一后台登录或登出面试系统</t>
   </si>
   <si>
+    <t xml:space="preserve">- 后端应当将HR，面试官，面试者都当做平台用户进行管理，记录他们的id和账户信息
+- 对于HR，后端应记录用户名、密码、邮箱等各项信息
+- 对于面试者和面试官，后端应当可以为他们生成账户，并把账户关联到他们的面试房间信息上
+- 前端登录时，后端应生成token返回给前端，以便权限管理，并设置超时时间，在超时后将用户登出</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API权限管理</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- 后端应当按照token处理API调用权限
+- HR具有管理后台所有API调用权限
+- 面试官应当只具有面试房间各项API权限，以及管理后台编辑题目，查看候选人信息API权限
+- 候选人应当只具有面试过程中作答用API的权限</t>
+  </si>
+  <si>
     <t xml:space="preserve">Author</t>
   </si>
   <si>
@@ -557,6 +630,9 @@
     <t xml:space="preserve">F_2</t>
   </si>
   <si>
+    <t xml:space="preserve">登陆页</t>
+  </si>
+  <si>
     <t xml:space="preserve">王澎</t>
   </si>
   <si>
@@ -642,6 +718,33 @@
   </si>
   <si>
     <t xml:space="preserve">F_28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_40</t>
   </si>
 </sst>
 </file>
@@ -651,7 +754,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -701,12 +804,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Noto Sans CJK SC Regular"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -834,10 +931,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="102.758139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="112.232558139535"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -939,21 +1035,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="18.953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="19.2"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="18.953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="19.5674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="81.9581395348837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="71.7441860465116"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="20.6744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="20.6744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="21.1674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="89.4651162790698"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="78.2697674418605"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1261,7 +1356,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_16</v>
@@ -1276,9 +1371,11 @@
       <c r="E17" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F17" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_17</v>
@@ -1287,15 +1384,17 @@
         <v>7</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>70</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_18</v>
@@ -1304,15 +1403,17 @@
         <v>7</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>73</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_19</v>
@@ -1321,15 +1422,17 @@
         <v>7</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>76</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_20</v>
@@ -1338,15 +1441,17 @@
         <v>9</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D21" s="0"/>
       <c r="E21" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>79</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_21</v>
@@ -1355,15 +1460,17 @@
         <v>9</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D22" s="0"/>
       <c r="E22" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_22</v>
@@ -1372,15 +1479,17 @@
         <v>9</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D23" s="0"/>
       <c r="E23" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>85</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_23</v>
@@ -1389,15 +1498,17 @@
         <v>9</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D24" s="0"/>
       <c r="E24" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>88</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_24</v>
@@ -1406,15 +1517,17 @@
         <v>9</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D25" s="0"/>
       <c r="E25" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>91</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_25</v>
@@ -1423,15 +1536,17 @@
         <v>9</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="F26" s="11"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_26</v>
@@ -1440,15 +1555,17 @@
         <v>9</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="F27" s="11"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_27</v>
@@ -1457,15 +1574,17 @@
         <v>9</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="F28" s="11"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_28</v>
@@ -1474,15 +1593,17 @@
         <v>9</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F29" s="11"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>103</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_29</v>
@@ -1491,15 +1612,17 @@
         <v>11</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="F30" s="11"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>106</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_30</v>
@@ -1508,15 +1631,17 @@
         <v>11</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="F31" s="11"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>109</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_31</v>
@@ -1525,15 +1650,17 @@
         <v>11</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="F32" s="11"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>112</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_32</v>
@@ -1542,15 +1669,17 @@
         <v>11</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="F33" s="11"/>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>115</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_33</v>
@@ -1559,15 +1688,17 @@
         <v>11</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="F34" s="11"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>118</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_34</v>
@@ -1576,15 +1707,17 @@
         <v>11</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="F35" s="11"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>121</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_35</v>
@@ -1593,13 +1726,15 @@
         <v>11</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="F36" s="11"/>
+        <v>124</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="36.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="str">
@@ -1610,14 +1745,14 @@
         <v>13</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="D37" s="0"/>
       <c r="E37" s="0" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="36.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1629,11 +1764,11 @@
         <v>13</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="D38" s="0"/>
       <c r="E38" s="0" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="F38" s="11" t="s">
         <v>59</v>
@@ -1648,14 +1783,17 @@
         <v>13</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>132</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="str">
         <f aca="false">"F_"&amp;(ROW()-1)</f>
         <v>F_39</v>
@@ -1664,13 +1802,27 @@
         <v>3</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="D40" s="0"/>
       <c r="E40" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="F40" s="11"/>
+        <v>135</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="70.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="str">
+        <f aca="false">"F_"&amp;(ROW()-1)</f>
+        <v>F_40</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>138</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1696,13 +1848,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8604651162791"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.4604651162791"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.7209302325581"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.2139534883721"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.0744186046512"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.7953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.0604651162791"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1713,16 +1864,16 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1757,18 +1908,17 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4883720930233"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="25.7209302325581"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.506976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.153488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8604651162791"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.9674418604651"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="28.0604651162791"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.5953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.9953488372093"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1779,128 +1929,149 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="D2" s="9" t="n">
         <v>4</v>
       </c>
+      <c r="E2" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="D3" s="9" t="n">
         <v>2</v>
       </c>
+      <c r="E3" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="D4" s="9" t="n">
         <v>4</v>
       </c>
+      <c r="E4" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="D5" s="9" t="n">
         <v>4</v>
       </c>
+      <c r="E5" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="D6" s="9" t="n">
         <v>4</v>
       </c>
+      <c r="E6" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="D7" s="9" t="n">
         <v>3</v>
       </c>
+      <c r="E7" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="D8" s="9" t="n">
         <v>3</v>
       </c>
+      <c r="E8" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="D10" s="9" t="n">
         <v>4</v>
@@ -1911,13 +2082,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="D11" s="9" t="n">
         <v>4</v>
@@ -1944,19 +2115,19 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.306976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.7674418604651"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.4883720930233"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8744186046512"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0604651162791"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.4279069767442"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7023255813953"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1967,255 +2138,306 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E2" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E3" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="E4" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E5" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E6" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E7" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="E9" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="E10" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E12" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E13" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="E14" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="E15" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>1.5</v>
       </c>
+      <c r="E16" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>1.5</v>
       </c>
+      <c r="E17" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>1.5</v>
       </c>
+      <c r="E18" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>1.5</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2242,15 +2464,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.9860465116279"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.7813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="32.8186046511628"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2261,86 +2487,195 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>78</v>
+        <v>84</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>80</v>
+        <v>87</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
+        <v>90</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>176</v>
+      </c>
       <c r="B11" s="12" t="s">
-        <v>92</v>
+        <v>105</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="B12" s="12" t="s">
-        <v>94</v>
+        <v>108</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>178</v>
+      </c>
       <c r="B13" s="12" t="s">
-        <v>96</v>
+        <v>111</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>179</v>
+      </c>
       <c r="B14" s="12" t="s">
-        <v>98</v>
+        <v>114</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="B15" s="12" t="s">
-        <v>100</v>
+        <v>117</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="B16" s="12" t="s">
-        <v>102</v>
+        <v>120</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="B17" s="12" t="s">
-        <v>104</v>
+        <v>123</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>183</v>
+      </c>
       <c r="B18" s="12" t="s">
-        <v>111</v>
+        <v>131</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>